<commit_message>
Added a BOM file and updated schematic and layout to address: Issue #7, Issue #6, Issue #5, Issue #4, Issue #3, Issue #2, Issue #1
</commit_message>
<xml_diff>
--- a/superDuino BOM.xlsx
+++ b/superDuino BOM.xlsx
@@ -422,7 +422,7 @@
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,11 +510,11 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>4.6399999999999997</v>
+        <v>3.4799999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -528,11 +528,11 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>4.6399999999999997</v>
+        <v>3.4799999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
       </c>
       <c r="E14">
         <f>SUM(E3:E12)</f>
-        <v>39.71</v>
+        <v>37.389999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
       </c>
       <c r="E18">
         <f>E16+E14</f>
-        <v>52.71</v>
+        <v>50.389999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>